<commit_message>
Update to some datasheets Mainly adding to .rmds - text primarily
</commit_message>
<xml_diff>
--- a/quality_scores_vals.xlsx
+++ b/quality_scores_vals.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t xml:space="preserve">Study</t>
   </si>
@@ -125,9 +125,6 @@
     <t xml:space="preserve">ACE</t>
   </si>
   <si>
-    <t xml:space="preserve">Han et al. (2013)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Karp et al. (2008)</t>
   </si>
   <si>
@@ -146,9 +143,6 @@
     <t xml:space="preserve">Ojeda et al. (2016)</t>
   </si>
   <si>
-    <t xml:space="preserve">TYM</t>
-  </si>
-  <si>
     <t xml:space="preserve">Oláh et al. (2020)</t>
   </si>
   <si>
@@ -201,6 +195,24 @@
   </si>
   <si>
     <t xml:space="preserve">Maneeton et al. (2010)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hamed et al. (2012)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baptista et al. (2017)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitturi et al. (2019)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peterson et al. (2018)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Güzel et al. (2018)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kotb et al. (2019)</t>
   </si>
 </sst>
 </file>
@@ -1122,16 +1134,14 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B17" t="n">
         <v>1</v>
       </c>
-      <c r="C17" t="n">
-        <v>1</v>
-      </c>
+      <c r="C17"/>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -1155,20 +1165,16 @@
         <v>1</v>
       </c>
       <c r="L17" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" t="n">
-        <v>1</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B18"/>
       <c r="C18"/>
-      <c r="D18" t="n">
-        <v>0</v>
-      </c>
+      <c r="D18"/>
       <c r="E18" t="n">
         <v>0</v>
       </c>
@@ -1179,7 +1185,7 @@
         <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" t="s">
         <v>13</v>
@@ -1191,30 +1197,36 @@
         <v>1</v>
       </c>
       <c r="L18" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
+        <v>33</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
       <c r="E19" t="n">
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J19" t="s">
         <v>14</v>
@@ -1223,16 +1235,14 @@
         <v>1</v>
       </c>
       <c r="L19" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" t="n">
-        <v>1</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B20"/>
       <c r="C20" t="n">
         <v>1</v>
       </c>
@@ -1246,7 +1256,7 @@
         <v>1</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" t="n">
         <v>1</v>
@@ -1266,9 +1276,11 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21"/>
+        <v>35</v>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
       <c r="C21" t="n">
         <v>1</v>
       </c>
@@ -1279,16 +1291,16 @@
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" t="n">
         <v>1</v>
       </c>
       <c r="H21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="J21" t="s">
         <v>14</v>
@@ -1297,12 +1309,12 @@
         <v>1</v>
       </c>
       <c r="L21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B22" t="n">
         <v>1</v>
@@ -1310,23 +1322,21 @@
       <c r="C22" t="n">
         <v>1</v>
       </c>
-      <c r="D22" t="n">
-        <v>0</v>
-      </c>
+      <c r="D22"/>
       <c r="E22" t="n">
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" t="n">
         <v>1</v>
       </c>
       <c r="H22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="J22" t="s">
         <v>14</v>
@@ -1335,15 +1345,15 @@
         <v>1</v>
       </c>
       <c r="L22" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" t="n">
         <v>1</v>
@@ -1352,17 +1362,15 @@
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
-      </c>
-      <c r="H23" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H23"/>
       <c r="I23" t="s">
         <v>13</v>
       </c>
@@ -1373,28 +1381,30 @@
         <v>1</v>
       </c>
       <c r="L23" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
         <v>1</v>
       </c>
-      <c r="D24"/>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
       <c r="E24" t="n">
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" t="n">
         <v>1</v>
@@ -1409,12 +1419,12 @@
         <v>1</v>
       </c>
       <c r="L24" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B25" t="n">
         <v>1</v>
@@ -1432,11 +1442,13 @@
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>1</v>
-      </c>
-      <c r="H25"/>
+        <v>0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1</v>
+      </c>
       <c r="I25" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J25" t="s">
         <v>14</v>
@@ -1450,13 +1462,13 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
@@ -1474,7 +1486,7 @@
         <v>1</v>
       </c>
       <c r="I26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J26" t="s">
         <v>14</v>
@@ -1488,7 +1500,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B27" t="n">
         <v>1</v>
@@ -1500,19 +1512,19 @@
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J27" t="s">
         <v>14</v>
@@ -1521,12 +1533,12 @@
         <v>1</v>
       </c>
       <c r="L27" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B28" t="n">
         <v>1</v>
@@ -1534,14 +1546,12 @@
       <c r="C28" t="n">
         <v>1</v>
       </c>
-      <c r="D28" t="n">
-        <v>0</v>
-      </c>
+      <c r="D28"/>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28" t="n">
         <v>0</v>
@@ -1550,7 +1560,7 @@
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J28" t="s">
         <v>14</v>
@@ -1559,36 +1569,34 @@
         <v>1</v>
       </c>
       <c r="L28" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29" t="n">
-        <v>1</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B29"/>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29" t="n">
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" t="n">
         <v>0</v>
       </c>
       <c r="H29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J29" t="s">
         <v>14</v>
@@ -1597,18 +1605,16 @@
         <v>1</v>
       </c>
       <c r="L29" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" t="n">
-        <v>1</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B30"/>
       <c r="C30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" t="n">
         <v>0</v>
@@ -1617,7 +1623,7 @@
         <v>1</v>
       </c>
       <c r="F30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" t="n">
         <v>1</v>
@@ -1635,12 +1641,12 @@
         <v>1</v>
       </c>
       <c r="L30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B31" t="n">
         <v>1</v>
@@ -1648,23 +1654,21 @@
       <c r="C31" t="n">
         <v>1</v>
       </c>
-      <c r="D31" t="n">
-        <v>0</v>
-      </c>
+      <c r="D31"/>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J31" t="s">
         <v>14</v>
@@ -1678,11 +1682,9 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" t="n">
-        <v>1</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="B32"/>
       <c r="C32" t="n">
         <v>1</v>
       </c>
@@ -1693,10 +1695,10 @@
         <v>1</v>
       </c>
       <c r="F32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H32" t="n">
         <v>0</v>
@@ -1711,24 +1713,24 @@
         <v>1</v>
       </c>
       <c r="L32" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B33" t="n">
         <v>1</v>
       </c>
       <c r="C33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33" t="n">
         <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F33" t="n">
         <v>0</v>
@@ -1737,10 +1739,10 @@
         <v>1</v>
       </c>
       <c r="H33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="J33" t="s">
         <v>14</v>
@@ -1749,18 +1751,16 @@
         <v>1</v>
       </c>
       <c r="L33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>43</v>
-      </c>
-      <c r="B34" t="n">
-        <v>1</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="B34"/>
       <c r="C34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" t="n">
         <v>0</v>
@@ -1769,16 +1769,16 @@
         <v>1</v>
       </c>
       <c r="F34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="J34" t="s">
         <v>14</v>
@@ -1787,12 +1787,12 @@
         <v>1</v>
       </c>
       <c r="L34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B35" t="n">
         <v>1</v>
@@ -1804,19 +1804,19 @@
         <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35" t="n">
         <v>1</v>
       </c>
       <c r="H35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J35" t="s">
         <v>14</v>
@@ -1825,12 +1825,12 @@
         <v>1</v>
       </c>
       <c r="L35" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B36" t="n">
         <v>1</v>
@@ -1838,21 +1838,23 @@
       <c r="C36" t="n">
         <v>1</v>
       </c>
-      <c r="D36"/>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
       <c r="E36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36" t="n">
         <v>1</v>
       </c>
       <c r="I36" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J36" t="s">
         <v>14</v>
@@ -1861,22 +1863,22 @@
         <v>1</v>
       </c>
       <c r="L36" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>46</v>
-      </c>
-      <c r="B37"/>
+        <v>52</v>
+      </c>
+      <c r="B37" t="n">
+        <v>1</v>
+      </c>
       <c r="C37" t="n">
         <v>1</v>
       </c>
-      <c r="D37" t="n">
-        <v>0</v>
-      </c>
+      <c r="D37"/>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F37" t="n">
         <v>1</v>
@@ -1885,7 +1887,7 @@
         <v>0</v>
       </c>
       <c r="H37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37" t="s">
         <v>13</v>
@@ -1897,16 +1899,18 @@
         <v>1</v>
       </c>
       <c r="L37" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>47</v>
-      </c>
-      <c r="B38"/>
+        <v>53</v>
+      </c>
+      <c r="B38" t="n">
+        <v>1</v>
+      </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" t="n">
         <v>0</v>
@@ -1915,11 +1919,9 @@
         <v>1</v>
       </c>
       <c r="F38" t="n">
-        <v>1</v>
-      </c>
-      <c r="G38" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G38"/>
       <c r="H38" t="n">
         <v>0</v>
       </c>
@@ -1938,20 +1940,22 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B39" t="n">
         <v>1</v>
       </c>
       <c r="C39" t="n">
-        <v>1</v>
-      </c>
-      <c r="D39"/>
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
       <c r="E39" t="n">
         <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G39" t="n">
         <v>0</v>
@@ -1960,7 +1964,7 @@
         <v>1</v>
       </c>
       <c r="I39" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J39" t="s">
         <v>14</v>
@@ -1969,34 +1973,34 @@
         <v>1</v>
       </c>
       <c r="L39" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B40"/>
       <c r="C40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40" t="n">
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F40" t="n">
         <v>1</v>
       </c>
       <c r="G40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J40" t="s">
         <v>14</v>
@@ -2010,7 +2014,7 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B41" t="n">
         <v>1</v>
@@ -2025,7 +2029,7 @@
         <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G41" t="n">
         <v>1</v>
@@ -2043,32 +2047,32 @@
         <v>1</v>
       </c>
       <c r="L41" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>51</v>
-      </c>
-      <c r="B42"/>
+        <v>57</v>
+      </c>
+      <c r="B42" t="n">
+        <v>1</v>
+      </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>0</v>
-      </c>
-      <c r="H42" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H42"/>
       <c r="I42" t="s">
         <v>13</v>
       </c>
@@ -2079,18 +2083,16 @@
         <v>1</v>
       </c>
       <c r="L42" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>52</v>
-      </c>
-      <c r="B43" t="n">
-        <v>1</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="B43"/>
       <c r="C43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D43" t="n">
         <v>0</v>
@@ -2099,16 +2101,14 @@
         <v>0</v>
       </c>
       <c r="F43" t="n">
-        <v>1</v>
-      </c>
-      <c r="G43" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G43"/>
       <c r="H43" t="n">
         <v>1</v>
       </c>
       <c r="I43" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="J43" t="s">
         <v>14</v>
@@ -2117,12 +2117,12 @@
         <v>1</v>
       </c>
       <c r="L43" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B44" t="n">
         <v>1</v>
@@ -2137,7 +2137,7 @@
         <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" t="n">
         <v>1</v>
@@ -2146,7 +2146,7 @@
         <v>1</v>
       </c>
       <c r="I44" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J44" t="s">
         <v>14</v>
@@ -2155,12 +2155,12 @@
         <v>1</v>
       </c>
       <c r="L44" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B45" t="n">
         <v>1</v>
@@ -2168,15 +2168,17 @@
       <c r="C45" t="n">
         <v>1</v>
       </c>
-      <c r="D45"/>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
       <c r="E45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
         <v>1</v>
       </c>
       <c r="G45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45" t="n">
         <v>1</v>
@@ -2191,19 +2193,17 @@
         <v>1</v>
       </c>
       <c r="L45" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B46" t="n">
         <v>1</v>
       </c>
-      <c r="C46" t="n">
-        <v>1</v>
-      </c>
+      <c r="C46"/>
       <c r="D46" t="n">
         <v>0</v>
       </c>
@@ -2211,11 +2211,13 @@
         <v>1</v>
       </c>
       <c r="F46" t="n">
-        <v>0</v>
-      </c>
-      <c r="G46"/>
+        <v>1</v>
+      </c>
+      <c r="G46" t="n">
+        <v>1</v>
+      </c>
       <c r="H46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I46" t="s">
         <v>13</v>
@@ -2227,30 +2229,30 @@
         <v>1</v>
       </c>
       <c r="L46" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B47" t="n">
         <v>1</v>
       </c>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47" t="n">
         <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H47" t="n">
         <v>1</v>
@@ -2265,36 +2267,34 @@
         <v>1</v>
       </c>
       <c r="L47" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B48" t="n">
         <v>1</v>
       </c>
       <c r="C48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48" t="n">
         <v>0</v>
       </c>
-      <c r="E48" t="n">
-        <v>0</v>
-      </c>
+      <c r="E48"/>
       <c r="F48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48" t="n">
         <v>1</v>
       </c>
       <c r="I48" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J48" t="s">
         <v>14</v>
@@ -2303,23 +2303,23 @@
         <v>1</v>
       </c>
       <c r="L48" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>57</v>
-      </c>
-      <c r="B49"/>
+        <v>64</v>
+      </c>
+      <c r="B49" t="n">
+        <v>1</v>
+      </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49" t="n">
-        <v>0</v>
-      </c>
-      <c r="E49" t="n">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E49"/>
       <c r="F49" t="n">
         <v>1</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>1</v>
       </c>
       <c r="I49" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J49" t="s">
         <v>14</v>
@@ -2339,12 +2339,12 @@
         <v>1</v>
       </c>
       <c r="L49" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B50" t="n">
         <v>1</v>
@@ -2355,14 +2355,12 @@
       <c r="D50" t="n">
         <v>0</v>
       </c>
-      <c r="E50" t="n">
-        <v>0</v>
-      </c>
+      <c r="E50"/>
       <c r="F50" t="n">
         <v>1</v>
       </c>
       <c r="G50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H50" t="n">
         <v>1</v>
@@ -2377,21 +2375,19 @@
         <v>1</v>
       </c>
       <c r="L50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>59</v>
-      </c>
-      <c r="B51" t="n">
-        <v>1</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="B51"/>
       <c r="C51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E51" t="n">
         <v>0</v>
@@ -2400,11 +2396,13 @@
         <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>1</v>
-      </c>
-      <c r="H51"/>
+        <v>0</v>
+      </c>
+      <c r="H51" t="n">
+        <v>1</v>
+      </c>
       <c r="I51" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J51" t="s">
         <v>14</v>
@@ -2413,16 +2411,16 @@
         <v>1</v>
       </c>
       <c r="L51" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="s">
-        <v>60</v>
-      </c>
-      <c r="B52"/>
+      <c r="A52"/>
+      <c r="B52" t="n">
+        <v>1</v>
+      </c>
       <c r="C52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52" t="n">
         <v>0</v>
@@ -2433,13 +2431,13 @@
       <c r="F52" t="n">
         <v>0</v>
       </c>
-      <c r="G52"/>
+      <c r="G52" t="n">
+        <v>0</v>
+      </c>
       <c r="H52" t="n">
         <v>1</v>
       </c>
-      <c r="I52" t="s">
-        <v>16</v>
-      </c>
+      <c r="I52"/>
       <c r="J52" t="s">
         <v>14</v>
       </c>
@@ -2447,83 +2445,7 @@
         <v>1</v>
       </c>
       <c r="L52" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="s">
-        <v>61</v>
-      </c>
-      <c r="B53" t="n">
-        <v>1</v>
-      </c>
-      <c r="C53" t="n">
-        <v>1</v>
-      </c>
-      <c r="D53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E53" t="n">
-        <v>0</v>
-      </c>
-      <c r="F53" t="n">
-        <v>1</v>
-      </c>
-      <c r="G53" t="n">
-        <v>1</v>
-      </c>
-      <c r="H53" t="n">
-        <v>1</v>
-      </c>
-      <c r="I53" t="s">
-        <v>16</v>
-      </c>
-      <c r="J53" t="s">
-        <v>14</v>
-      </c>
-      <c r="K53" t="n">
-        <v>1</v>
-      </c>
-      <c r="L53" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="s">
-        <v>62</v>
-      </c>
-      <c r="B54" t="n">
-        <v>1</v>
-      </c>
-      <c r="C54" t="n">
-        <v>1</v>
-      </c>
-      <c r="D54" t="n">
-        <v>0</v>
-      </c>
-      <c r="E54" t="n">
-        <v>1</v>
-      </c>
-      <c r="F54" t="n">
-        <v>1</v>
-      </c>
-      <c r="G54" t="n">
-        <v>1</v>
-      </c>
-      <c r="H54" t="n">
-        <v>1</v>
-      </c>
-      <c r="I54" t="s">
-        <v>13</v>
-      </c>
-      <c r="J54" t="s">
-        <v>14</v>
-      </c>
-      <c r="K54" t="n">
-        <v>1</v>
-      </c>
-      <c r="L54" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>